<commit_message>
Splitting type-specific tests to be more individual, and including a test for multiple types, as well as modifying the Excel file to include more mixed data.
</commit_message>
<xml_diff>
--- a/tests/ExcelProvider.Tests/MixedDataTypes.xlsx
+++ b/tests/ExcelProvider.Tests/MixedDataTypes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Repositories\fSharp\ExcelProvider\tests\ExcelProvider.Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19320B45-8B17-4C9F-A9AF-A5EC98FC308F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C60CE7A-D19E-4B4E-8A0B-4B3291E5033D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24480" yWindow="2355" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>Title</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>$418 million</t>
+  </si>
+  <si>
+    <t>Date Watched</t>
+  </si>
+  <si>
+    <t>2013-01-25</t>
   </si>
 </sst>
 </file>
@@ -167,7 +173,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -198,11 +204,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -484,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,9 +506,10 @@
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -523,12 +531,15 @@
       <c r="G1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2">
         <v>1996</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -546,12 +557,15 @@
       <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="4">
+        <v>36194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>1975</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -569,12 +583,15 @@
       <c r="G3" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="1">
+        <v>39160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1984</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <v>1956</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -590,12 +607,15 @@
       <c r="G4" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="4">
+        <v>44330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.45</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5">
         <v>2007</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -609,12 +629,15 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>1968</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -632,12 +655,15 @@
       <c r="G6" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="4">
+        <v>36892</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2012</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>2009</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -655,12 +681,15 @@
       <c r="G7" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="2">
+        <v>40768</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>300</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="1">
         <v>2006</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -678,12 +707,15 @@
       <c r="G8" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="4">
+        <v>39132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="1">
         <v>2007</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -697,12 +729,15 @@
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="5">
+        <v>43071</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="1">
         <v>1937</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -719,6 +754,9 @@
       </c>
       <c r="G10" s="3" t="s">
         <v>44</v>
+      </c>
+      <c r="H10" s="4">
+        <v>35749</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Doing a better job of testing, including: Actually marking your test functions as tests
</commit_message>
<xml_diff>
--- a/tests/ExcelProvider.Tests/MixedDataTypes.xlsx
+++ b/tests/ExcelProvider.Tests/MixedDataTypes.xlsx
@@ -8,24 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Repositories\fSharp\ExcelProvider\tests\ExcelProvider.Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C60CE7A-D19E-4B4E-8A0B-4B3291E5033D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6660A8-20ED-4C50-9FC5-DEED210EFA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24480" yWindow="2355" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidDataTypes" sheetId="1" r:id="rId1"/>
+    <sheet name="InvalidDataTypes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="49">
   <si>
     <t>Title</t>
   </si>
@@ -166,6 +178,12 @@
   </si>
   <si>
     <t>2013-01-25</t>
+  </si>
+  <si>
+    <t>Nineteen Ninety Nine</t>
+  </si>
+  <si>
+    <t>$42 billion</t>
   </si>
 </sst>
 </file>
@@ -494,7 +512,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +576,8 @@
         <v>13</v>
       </c>
       <c r="H2" s="4">
-        <v>36194</v>
+        <f ca="1">TODAY()</f>
+        <v>45532</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -762,4 +781,232 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75DA43EE-4359-412B-B240-31D611B73112}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1996</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4">
+        <f ca="1">TODAY()</f>
+        <v>45532</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1984</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1956</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="4">
+        <v>44330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.45</v>
+      </c>
+      <c r="B5" s="4">
+        <v>44330</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>1968</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="4">
+        <v>36892</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2012</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>